<commit_message>
Work on grade reports and tables
</commit_message>
<xml_diff>
--- a/TestData/Schuljahre/SCHULJAHR_2016/Noten_2/Noten_10.xlsx
+++ b/TestData/Schuljahre/SCHULJAHR_2016/Noten_2/Noten_10.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -52,6 +52,13 @@
       <charset val="1"/>
       <family val="0"/>
       <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="12"/>
     </font>
@@ -117,7 +124,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -127,25 +134,28 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="8" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
@@ -154,13 +164,13 @@
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" textRotation="90" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="2" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" applyProtection="1" borderId="2" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
@@ -175,22 +185,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="8" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
@@ -199,13 +212,13 @@
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" textRotation="90" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="2" fillId="0" fontId="6" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" applyProtection="1" borderId="2" fillId="0" fontId="7" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
@@ -513,1328 +526,1351 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="E9" xSplit="4" ySplit="8"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="E1" activeCellId="0" pane="topRight" sqref="E1"/>
-      <selection activeCell="A9" activeCellId="0" pane="bottomLeft" sqref="A9"/>
-      <selection activeCell="B9" activeCellId="0" pane="bottomRight" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="10"/>
-    <col customWidth="1" max="2" min="2" style="15" width="26.74"/>
-    <col customWidth="1" max="3" min="3" style="15" width="11.81"/>
-    <col customWidth="1" max="4" min="4" style="15" width="1.51"/>
-    <col customWidth="1" max="26" min="5" style="15" width="7.49"/>
-    <col customWidth="1" max="30" min="27" style="15" width="7.65"/>
-    <col customWidth="1" max="1007" min="31" style="15" width="8.67"/>
-    <col customWidth="1" max="1025" min="1008" style="15" width="11.52"/>
+    <col customWidth="1" max="1" min="1" style="16" width="10"/>
+    <col customWidth="1" max="2" min="2" style="16" width="26.74"/>
+    <col customWidth="1" max="3" min="3" style="16" width="11.81"/>
+    <col customWidth="1" max="4" min="4" style="16" width="1.51"/>
+    <col customWidth="1" max="26" min="5" style="16" width="7.49"/>
+    <col customWidth="1" max="30" min="27" style="16" width="7.65"/>
+    <col customWidth="1" max="1007" min="31" style="16" width="8.67"/>
+    <col customWidth="1" max="1025" min="1008" style="16" width="11.52"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="28" r="1" s="16">
-      <c r="A1" s="17" t="n"/>
-      <c r="B1" s="18" t="inlineStr">
-        <is>
-          <t>Noten zu 2020-03-16 09:25</t>
-        </is>
-      </c>
-      <c r="C1" s="19" t="n"/>
-      <c r="D1" s="19" t="n"/>
+    <row customHeight="1" ht="28" r="1" s="17">
+      <c r="A1" s="18" t="n"/>
+      <c r="B1" s="19" t="inlineStr">
+        <is>
+          <t>Noten, Konferenz am 13.06.2016</t>
+        </is>
+      </c>
+      <c r="C1" s="20" t="n"/>
+      <c r="D1" s="20" t="n"/>
+      <c r="F1" s="21" t="inlineStr">
+        <is>
+          <t>Tabelle erstellt am 2020-03-21 07:24</t>
+        </is>
+      </c>
+      <c r="G1" s="20" t="n"/>
+      <c r="H1" s="20" t="n"/>
+      <c r="I1" s="20" t="n"/>
+      <c r="J1" s="20" t="n"/>
+      <c r="K1" s="20" t="n"/>
+      <c r="L1" s="20" t="n"/>
+      <c r="M1" s="20" t="n"/>
+      <c r="N1" s="20" t="n"/>
+      <c r="O1" s="20" t="n"/>
+      <c r="P1" s="20" t="n"/>
+      <c r="Q1" s="20" t="n"/>
+      <c r="R1" s="20" t="n"/>
+      <c r="S1" s="20" t="n"/>
     </row>
-    <row customHeight="1" ht="22.4" r="2" s="16">
-      <c r="A2" s="20" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="2" s="17">
+      <c r="A2" s="22" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B2" s="20" t="inlineStr">
+      <c r="B2" s="22" t="inlineStr">
         <is>
           <t>Schuljahr</t>
         </is>
       </c>
-      <c r="C2" s="20" t="inlineStr">
+      <c r="C2" s="22" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
       </c>
-      <c r="D2" s="20" t="n"/>
-      <c r="E2" s="20" t="n"/>
-      <c r="F2" s="20" t="inlineStr">
+      <c r="D2" s="22" t="n"/>
+      <c r="E2" s="22" t="n"/>
+      <c r="F2" s="22" t="inlineStr">
         <is>
           <t>Noten im Bereich 1–6.  [+ und - dürfen angegeben werden, obwohl diese nicht im Zeugnis erscheinen.]</t>
         </is>
       </c>
-      <c r="T2" s="20" t="n"/>
-      <c r="U2" s="20" t="n"/>
+      <c r="T2" s="22" t="n"/>
+      <c r="U2" s="22" t="n"/>
     </row>
-    <row customHeight="1" ht="22.4" r="3" s="16">
-      <c r="A3" s="20" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="3" s="17">
+      <c r="A3" s="22" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B3" s="20" t="inlineStr">
+      <c r="B3" s="22" t="inlineStr">
         <is>
           <t>Klasse</t>
         </is>
       </c>
-      <c r="C3" s="20" t="inlineStr">
+      <c r="C3" s="22" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="D3" s="20" t="n"/>
-      <c r="E3" s="20" t="n"/>
-      <c r="F3" s="20" t="inlineStr">
+      <c r="D3" s="22" t="n"/>
+      <c r="E3" s="22" t="n"/>
+      <c r="F3" s="22" t="inlineStr">
         <is>
           <t>Auch möglich sind:</t>
         </is>
       </c>
-      <c r="I3" s="21" t="inlineStr">
+      <c r="I3" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">nt: </t>
         </is>
       </c>
-      <c r="J3" s="20" t="inlineStr">
+      <c r="J3" s="22" t="inlineStr">
         <is>
           <t>nicht teilgenommen</t>
         </is>
       </c>
-      <c r="M3" s="21" t="inlineStr">
+      <c r="M3" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">nb: </t>
         </is>
       </c>
-      <c r="N3" s="20" t="inlineStr">
+      <c r="N3" s="22" t="inlineStr">
         <is>
           <t>nicht bewertbar</t>
         </is>
       </c>
-      <c r="Q3" s="20" t="n"/>
-      <c r="R3" s="20" t="n"/>
-      <c r="S3" s="20" t="n"/>
-      <c r="U3" s="20" t="n"/>
+      <c r="Q3" s="23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">*: </t>
+        </is>
+      </c>
+      <c r="R3" s="22" t="inlineStr">
+        <is>
+          <t>keine Note</t>
+        </is>
+      </c>
+      <c r="U3" s="22" t="n"/>
     </row>
-    <row customHeight="1" ht="22.4" r="4" s="16">
-      <c r="A4" s="20" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="4" s="17">
+      <c r="A4" s="22" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B4" s="20" t="inlineStr">
+      <c r="B4" s="22" t="inlineStr">
         <is>
           <t>Halbjahr</t>
         </is>
       </c>
-      <c r="C4" s="20" t="inlineStr">
+      <c r="C4" s="22" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D4" s="20" t="n"/>
-      <c r="E4" s="20" t="n"/>
-      <c r="F4" s="20" t="n"/>
-      <c r="G4" s="20" t="n"/>
-      <c r="H4" s="20" t="n"/>
-      <c r="I4" s="22" t="inlineStr">
+      <c r="D4" s="22" t="n"/>
+      <c r="E4" s="22" t="n"/>
+      <c r="F4" s="22" t="n"/>
+      <c r="G4" s="22" t="n"/>
+      <c r="H4" s="22" t="n"/>
+      <c r="I4" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">t: </t>
         </is>
       </c>
-      <c r="J4" s="23" t="inlineStr">
+      <c r="J4" s="25" t="inlineStr">
         <is>
           <t>teilgenommen</t>
         </is>
       </c>
-      <c r="M4" s="24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">*: </t>
-        </is>
-      </c>
-      <c r="N4" s="23" t="inlineStr">
+      <c r="M4" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">/: </t>
+        </is>
+      </c>
+      <c r="N4" s="25" t="inlineStr">
         <is>
           <t>Fach nicht gewählt / nicht erteilt</t>
         </is>
       </c>
-      <c r="U4" s="20" t="n"/>
+      <c r="U4" s="22" t="n"/>
     </row>
-    <row customHeight="1" ht="8.4" r="5" s="16"/>
-    <row customHeight="1" ht="44.8" r="6" s="16">
-      <c r="A6" s="25" t="inlineStr">
+    <row customHeight="1" ht="8.4" r="5" s="17"/>
+    <row customHeight="1" ht="44.8" r="6" s="17">
+      <c r="A6" s="27" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B6" s="25" t="inlineStr">
+      <c r="B6" s="27" t="inlineStr">
         <is>
           <t>Schüler(in)</t>
         </is>
       </c>
-      <c r="C6" s="25" t="inlineStr">
+      <c r="C6" s="27" t="inlineStr">
         <is>
           <t>Maßstab</t>
         </is>
       </c>
-      <c r="D6" s="26" t="n"/>
-      <c r="E6" s="25" t="inlineStr">
+      <c r="D6" s="28" t="n"/>
+      <c r="E6" s="27" t="inlineStr">
         <is>
           <t>De</t>
         </is>
       </c>
-      <c r="F6" s="25" t="inlineStr">
+      <c r="F6" s="27" t="inlineStr">
         <is>
           <t>En</t>
         </is>
       </c>
-      <c r="G6" s="25" t="inlineStr">
+      <c r="G6" s="27" t="inlineStr">
         <is>
           <t>Fr</t>
         </is>
       </c>
-      <c r="H6" s="25" t="inlineStr">
+      <c r="H6" s="27" t="inlineStr">
         <is>
           <t>Mu</t>
         </is>
       </c>
-      <c r="I6" s="25" t="inlineStr">
+      <c r="I6" s="27" t="inlineStr">
         <is>
           <t>Ges</t>
         </is>
       </c>
-      <c r="J6" s="25" t="inlineStr">
+      <c r="J6" s="27" t="inlineStr">
         <is>
           <t>Soz</t>
         </is>
       </c>
-      <c r="K6" s="25" t="inlineStr">
+      <c r="K6" s="27" t="inlineStr">
         <is>
           <t>Geo</t>
         </is>
       </c>
-      <c r="L6" s="25" t="inlineStr">
+      <c r="L6" s="27" t="inlineStr">
         <is>
           <t>Rel</t>
         </is>
       </c>
-      <c r="M6" s="25" t="inlineStr">
+      <c r="M6" s="27" t="inlineStr">
         <is>
           <t>Ma</t>
         </is>
       </c>
-      <c r="N6" s="25" t="inlineStr">
+      <c r="N6" s="27" t="inlineStr">
         <is>
           <t>Bio</t>
         </is>
       </c>
-      <c r="O6" s="25" t="inlineStr">
+      <c r="O6" s="27" t="inlineStr">
         <is>
           <t>Ch</t>
         </is>
       </c>
-      <c r="P6" s="25" t="inlineStr">
+      <c r="P6" s="27" t="inlineStr">
         <is>
           <t>AWT</t>
         </is>
       </c>
-      <c r="Q6" s="25" t="inlineStr">
+      <c r="Q6" s="27" t="inlineStr">
         <is>
           <t>Sp</t>
         </is>
       </c>
-      <c r="R6" s="25" t="inlineStr">
+      <c r="R6" s="27" t="inlineStr">
         <is>
           <t>Eu_</t>
         </is>
       </c>
-      <c r="S6" s="25" t="inlineStr">
+      <c r="S6" s="27" t="inlineStr">
         <is>
           <t>Ktr_k</t>
         </is>
       </c>
-      <c r="T6" s="25" t="inlineStr">
+      <c r="T6" s="27" t="inlineStr">
         <is>
           <t>Snt_k</t>
         </is>
       </c>
-      <c r="U6" s="25" t="inlineStr">
+      <c r="U6" s="27" t="inlineStr">
         <is>
           <t>Web_k</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="94.2" r="7" s="16">
-      <c r="A7" s="27" t="n"/>
-      <c r="B7" s="27" t="n"/>
-      <c r="C7" s="27" t="n"/>
-      <c r="D7" s="26" t="n"/>
-      <c r="E7" s="28" t="inlineStr">
+    <row customHeight="1" ht="94.2" r="7" s="17">
+      <c r="A7" s="29" t="n"/>
+      <c r="B7" s="29" t="n"/>
+      <c r="C7" s="29" t="n"/>
+      <c r="D7" s="28" t="n"/>
+      <c r="E7" s="30" t="inlineStr">
         <is>
           <t>Deutsch</t>
         </is>
       </c>
-      <c r="F7" s="28" t="inlineStr">
+      <c r="F7" s="30" t="inlineStr">
         <is>
           <t>Englisch</t>
         </is>
       </c>
-      <c r="G7" s="28" t="inlineStr">
+      <c r="G7" s="30" t="inlineStr">
         <is>
           <t>Französisch</t>
         </is>
       </c>
-      <c r="H7" s="28" t="inlineStr">
+      <c r="H7" s="30" t="inlineStr">
         <is>
           <t>Musik</t>
         </is>
       </c>
-      <c r="I7" s="28" t="inlineStr">
+      <c r="I7" s="30" t="inlineStr">
         <is>
           <t>Geschichte</t>
         </is>
       </c>
-      <c r="J7" s="28" t="inlineStr">
+      <c r="J7" s="30" t="inlineStr">
         <is>
           <t>Sozialkunde</t>
         </is>
       </c>
-      <c r="K7" s="28" t="inlineStr">
+      <c r="K7" s="30" t="inlineStr">
         <is>
           <t>Geographie</t>
         </is>
       </c>
-      <c r="L7" s="28" t="inlineStr">
+      <c r="L7" s="30" t="inlineStr">
         <is>
           <t>Religion</t>
         </is>
       </c>
-      <c r="M7" s="28" t="inlineStr">
+      <c r="M7" s="30" t="inlineStr">
         <is>
           <t>Mathematik</t>
         </is>
       </c>
-      <c r="N7" s="28" t="inlineStr">
+      <c r="N7" s="30" t="inlineStr">
         <is>
           <t>Biologie</t>
         </is>
       </c>
-      <c r="O7" s="28" t="inlineStr">
+      <c r="O7" s="30" t="inlineStr">
         <is>
           <t>Chemie</t>
         </is>
       </c>
-      <c r="P7" s="28" t="inlineStr">
+      <c r="P7" s="30" t="inlineStr">
         <is>
           <t>Arbeit-Wirtschaft-Technik</t>
         </is>
       </c>
-      <c r="Q7" s="28" t="inlineStr">
+      <c r="Q7" s="30" t="inlineStr">
         <is>
           <t>Sport</t>
         </is>
       </c>
-      <c r="R7" s="28" t="inlineStr">
+      <c r="R7" s="30" t="inlineStr">
         <is>
           <t>Eurythmie</t>
         </is>
       </c>
-      <c r="S7" s="28" t="inlineStr">
+      <c r="S7" s="30" t="inlineStr">
         <is>
           <t>Kupfertreiben</t>
         </is>
       </c>
-      <c r="T7" s="28" t="inlineStr">
+      <c r="T7" s="30" t="inlineStr">
         <is>
           <t>Schnitzen</t>
         </is>
       </c>
-      <c r="U7" s="28" t="inlineStr">
+      <c r="U7" s="30" t="inlineStr">
         <is>
           <t>Weben</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="8.4" r="8" s="16">
-      <c r="A8" s="26" t="n"/>
-      <c r="B8" s="26" t="n"/>
-      <c r="C8" s="26" t="n"/>
-      <c r="D8" s="26" t="n"/>
-      <c r="E8" s="26" t="n"/>
-      <c r="F8" s="26" t="n"/>
-      <c r="G8" s="26" t="n"/>
-      <c r="H8" s="26" t="n"/>
-      <c r="I8" s="26" t="n"/>
-      <c r="J8" s="26" t="n"/>
-      <c r="K8" s="26" t="n"/>
-      <c r="L8" s="26" t="n"/>
-      <c r="M8" s="26" t="n"/>
-      <c r="N8" s="26" t="n"/>
-      <c r="O8" s="26" t="n"/>
-      <c r="P8" s="26" t="n"/>
-      <c r="Q8" s="26" t="n"/>
-      <c r="R8" s="26" t="n"/>
-      <c r="S8" s="26" t="n"/>
-      <c r="T8" s="26" t="n"/>
-      <c r="U8" s="26" t="n"/>
+    <row customHeight="1" ht="8.4" r="8" s="17">
+      <c r="A8" s="28" t="n"/>
+      <c r="B8" s="28" t="n"/>
+      <c r="C8" s="28" t="n"/>
+      <c r="D8" s="28" t="n"/>
+      <c r="E8" s="28" t="n"/>
+      <c r="F8" s="28" t="n"/>
+      <c r="G8" s="28" t="n"/>
+      <c r="H8" s="28" t="n"/>
+      <c r="I8" s="28" t="n"/>
+      <c r="J8" s="28" t="n"/>
+      <c r="K8" s="28" t="n"/>
+      <c r="L8" s="28" t="n"/>
+      <c r="M8" s="28" t="n"/>
+      <c r="N8" s="28" t="n"/>
+      <c r="O8" s="28" t="n"/>
+      <c r="P8" s="28" t="n"/>
+      <c r="Q8" s="28" t="n"/>
+      <c r="R8" s="28" t="n"/>
+      <c r="S8" s="28" t="n"/>
+      <c r="T8" s="28" t="n"/>
+      <c r="U8" s="28" t="n"/>
     </row>
-    <row customHeight="1" ht="22.4" r="9" s="16">
-      <c r="A9" s="25" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="9" s="17">
+      <c r="A9" s="27" t="inlineStr">
         <is>
           <t>200601</t>
         </is>
       </c>
-      <c r="B9" s="29" t="inlineStr">
+      <c r="B9" s="31" t="inlineStr">
         <is>
           <t>Annegret Adelig</t>
         </is>
       </c>
-      <c r="C9" s="29" t="inlineStr">
+      <c r="C9" s="31" t="inlineStr">
         <is>
           <t>Gym</t>
         </is>
       </c>
-      <c r="D9" s="26" t="n"/>
-      <c r="E9" s="30" t="inlineStr">
+      <c r="D9" s="28" t="n"/>
+      <c r="E9" s="32" t="inlineStr">
         <is>
           <t>2+</t>
         </is>
       </c>
-      <c r="F9" s="30" t="inlineStr">
+      <c r="F9" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G9" s="30" t="inlineStr">
+      <c r="G9" s="32" t="inlineStr">
         <is>
           <t>1+</t>
         </is>
       </c>
-      <c r="H9" s="30" t="inlineStr">
+      <c r="H9" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I9" s="30" t="inlineStr">
+      <c r="I9" s="32" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="J9" s="30" t="inlineStr">
+      <c r="J9" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="K9" s="30" t="inlineStr">
+      <c r="K9" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="L9" s="30" t="inlineStr">
+      <c r="L9" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="M9" s="30" t="inlineStr">
+      <c r="M9" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="N9" s="30" t="inlineStr">
+      <c r="N9" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="O9" s="30" t="inlineStr">
+      <c r="O9" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="P9" s="30" t="inlineStr">
+      <c r="P9" s="32" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="Q9" s="30" t="inlineStr">
+      <c r="Q9" s="32" t="inlineStr">
         <is>
           <t>3+</t>
         </is>
       </c>
-      <c r="R9" s="30" t="inlineStr">
+      <c r="R9" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="S9" s="30" t="inlineStr">
+      <c r="S9" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
-      <c r="T9" s="30" t="inlineStr">
+      <c r="T9" s="32" t="inlineStr">
         <is>
           <t>nb</t>
         </is>
       </c>
-      <c r="U9" s="30" t="inlineStr">
+      <c r="U9" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22.4" r="10" s="16">
-      <c r="A10" s="25" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="10" s="17">
+      <c r="A10" s="27" t="inlineStr">
         <is>
           <t>200602</t>
         </is>
       </c>
-      <c r="B10" s="29" t="inlineStr">
+      <c r="B10" s="31" t="inlineStr">
         <is>
           <t>Bertha Bunte</t>
         </is>
       </c>
-      <c r="C10" s="29" t="inlineStr">
+      <c r="C10" s="31" t="inlineStr">
         <is>
           <t>Gym</t>
         </is>
       </c>
-      <c r="D10" s="26" t="n"/>
-      <c r="E10" s="30" t="inlineStr">
+      <c r="D10" s="28" t="n"/>
+      <c r="E10" s="32" t="inlineStr">
         <is>
           <t>1+</t>
         </is>
       </c>
-      <c r="F10" s="30" t="inlineStr">
+      <c r="F10" s="32" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="G10" s="30" t="inlineStr">
+      <c r="G10" s="32" t="inlineStr">
         <is>
           <t>2+</t>
         </is>
       </c>
-      <c r="H10" s="30" t="inlineStr">
+      <c r="H10" s="32" t="inlineStr">
         <is>
           <t>2+</t>
         </is>
       </c>
-      <c r="I10" s="30" t="inlineStr">
+      <c r="I10" s="32" t="inlineStr">
         <is>
           <t>3+</t>
         </is>
       </c>
-      <c r="J10" s="30" t="inlineStr">
+      <c r="J10" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="K10" s="30" t="inlineStr">
+      <c r="K10" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="L10" s="30" t="inlineStr">
+      <c r="L10" s="32" t="inlineStr">
         <is>
           <t>2+</t>
         </is>
       </c>
-      <c r="M10" s="30" t="inlineStr">
+      <c r="M10" s="32" t="inlineStr">
         <is>
           <t>1-</t>
         </is>
       </c>
-      <c r="N10" s="30" t="inlineStr">
+      <c r="N10" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="O10" s="30" t="inlineStr">
+      <c r="O10" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="P10" s="30" t="inlineStr">
+      <c r="P10" s="32" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="Q10" s="30" t="inlineStr">
+      <c r="Q10" s="32" t="inlineStr">
         <is>
           <t>1-</t>
         </is>
       </c>
-      <c r="R10" s="30" t="inlineStr">
+      <c r="R10" s="32" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="S10" s="30" t="inlineStr">
+      <c r="S10" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="T10" s="30" t="inlineStr">
+      <c r="T10" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
-      <c r="U10" s="30" t="inlineStr">
+      <c r="U10" s="32" t="inlineStr">
         <is>
           <t>1+</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22.4" r="11" s="16">
-      <c r="A11" s="25" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="11" s="17">
+      <c r="A11" s="27" t="inlineStr">
         <is>
           <t>200603</t>
         </is>
       </c>
-      <c r="B11" s="29" t="inlineStr">
+      <c r="B11" s="31" t="inlineStr">
         <is>
           <t>Christian Carstensen</t>
         </is>
       </c>
-      <c r="C11" s="29" t="inlineStr">
+      <c r="C11" s="31" t="inlineStr">
         <is>
           <t>Gym</t>
         </is>
       </c>
-      <c r="D11" s="26" t="n"/>
-      <c r="E11" s="30" t="inlineStr">
+      <c r="D11" s="28" t="n"/>
+      <c r="E11" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="F11" s="30" t="inlineStr">
+      <c r="F11" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G11" s="30" t="inlineStr">
+      <c r="G11" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="H11" s="30" t="inlineStr">
+      <c r="H11" s="32" t="inlineStr">
         <is>
           <t>3+</t>
         </is>
       </c>
-      <c r="I11" s="30" t="inlineStr">
+      <c r="I11" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="J11" s="30" t="inlineStr">
+      <c r="J11" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="K11" s="30" t="n"/>
-      <c r="L11" s="30" t="inlineStr">
+      <c r="K11" s="32" t="n"/>
+      <c r="L11" s="32" t="inlineStr">
         <is>
           <t>nb</t>
         </is>
       </c>
-      <c r="M11" s="30" t="inlineStr">
+      <c r="M11" s="32" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="N11" s="30" t="inlineStr">
+      <c r="N11" s="32" t="inlineStr">
         <is>
           <t>4+</t>
         </is>
       </c>
-      <c r="O11" s="30" t="inlineStr">
+      <c r="O11" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="P11" s="30" t="inlineStr">
+      <c r="P11" s="32" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="Q11" s="30" t="inlineStr">
+      <c r="Q11" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="R11" s="30" t="inlineStr">
+      <c r="R11" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="S11" s="30" t="inlineStr">
+      <c r="S11" s="32" t="inlineStr">
         <is>
           <t>1-</t>
         </is>
       </c>
-      <c r="T11" s="30" t="inlineStr">
+      <c r="T11" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
-      <c r="U11" s="30" t="inlineStr">
+      <c r="U11" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22.4" r="12" s="16">
-      <c r="A12" s="25" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="12" s="17">
+      <c r="A12" s="27" t="inlineStr">
         <is>
           <t>200604</t>
         </is>
       </c>
-      <c r="B12" s="29" t="inlineStr">
+      <c r="B12" s="31" t="inlineStr">
         <is>
           <t>David Dämmermann</t>
         </is>
       </c>
-      <c r="C12" s="29" t="inlineStr">
+      <c r="C12" s="31" t="inlineStr">
         <is>
           <t>Gym</t>
         </is>
       </c>
-      <c r="D12" s="26" t="n"/>
-      <c r="E12" s="30" t="inlineStr">
+      <c r="D12" s="28" t="n"/>
+      <c r="E12" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="F12" s="30" t="inlineStr">
+      <c r="F12" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G12" s="30" t="inlineStr">
+      <c r="G12" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="H12" s="30" t="inlineStr">
+      <c r="H12" s="32" t="inlineStr">
         <is>
           <t>5+</t>
         </is>
       </c>
-      <c r="I12" s="30" t="inlineStr">
+      <c r="I12" s="32" t="inlineStr">
         <is>
           <t>4+</t>
         </is>
       </c>
-      <c r="J12" s="30" t="inlineStr">
+      <c r="J12" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="K12" s="30" t="inlineStr">
+      <c r="K12" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="L12" s="30" t="inlineStr">
+      <c r="L12" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="M12" s="30" t="inlineStr">
+      <c r="M12" s="32" t="inlineStr">
         <is>
           <t>5-</t>
         </is>
       </c>
-      <c r="N12" s="30" t="inlineStr">
+      <c r="N12" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="O12" s="30" t="inlineStr">
+      <c r="O12" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="P12" s="30" t="inlineStr">
+      <c r="P12" s="32" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="Q12" s="30" t="inlineStr">
+      <c r="Q12" s="32" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="R12" s="30" t="inlineStr">
+      <c r="R12" s="32" t="inlineStr">
         <is>
           <t>5-</t>
         </is>
       </c>
-      <c r="S12" s="30" t="inlineStr">
+      <c r="S12" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
-      <c r="T12" s="30" t="inlineStr">
+      <c r="T12" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
-      <c r="U12" s="30" t="inlineStr">
+      <c r="U12" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22.4" r="13" s="16">
-      <c r="A13" s="25" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="13" s="17">
+      <c r="A13" s="27" t="inlineStr">
         <is>
           <t>200951</t>
         </is>
       </c>
-      <c r="B13" s="29" t="inlineStr">
+      <c r="B13" s="31" t="inlineStr">
         <is>
           <t>Ole zu den Erlen</t>
         </is>
       </c>
-      <c r="C13" s="29" t="inlineStr">
+      <c r="C13" s="31" t="inlineStr">
         <is>
           <t>RS</t>
         </is>
       </c>
-      <c r="D13" s="26" t="n"/>
-      <c r="E13" s="30" t="inlineStr">
+      <c r="D13" s="28" t="n"/>
+      <c r="E13" s="32" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="F13" s="30" t="inlineStr">
+      <c r="F13" s="32" t="inlineStr">
         <is>
           <t>5-</t>
         </is>
       </c>
-      <c r="G13" s="30" t="inlineStr">
+      <c r="G13" s="32" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="H13" s="30" t="inlineStr">
+      <c r="H13" s="32" t="inlineStr">
         <is>
           <t>3+</t>
         </is>
       </c>
-      <c r="I13" s="30" t="inlineStr">
+      <c r="I13" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="J13" s="30" t="inlineStr">
+      <c r="J13" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="K13" s="30" t="inlineStr">
+      <c r="K13" s="32" t="inlineStr">
         <is>
           <t>nb</t>
         </is>
       </c>
-      <c r="L13" s="30" t="inlineStr">
+      <c r="L13" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
-      <c r="M13" s="30" t="inlineStr">
+      <c r="M13" s="32" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="N13" s="30" t="inlineStr">
+      <c r="N13" s="32" t="inlineStr">
         <is>
           <t>4+</t>
         </is>
       </c>
-      <c r="O13" s="30" t="inlineStr">
+      <c r="O13" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="P13" s="30" t="n"/>
-      <c r="Q13" s="30" t="inlineStr">
+      <c r="P13" s="32" t="n"/>
+      <c r="Q13" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="R13" s="30" t="inlineStr">
+      <c r="R13" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="S13" s="30" t="inlineStr">
+      <c r="S13" s="32" t="inlineStr">
         <is>
           <t>1-</t>
         </is>
       </c>
-      <c r="T13" s="30" t="inlineStr">
+      <c r="T13" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="U13" s="30" t="inlineStr">
+      <c r="U13" s="32" t="inlineStr">
         <is>
           <t>2+</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22.4" r="14" s="16">
-      <c r="A14" s="25" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="14" s="17">
+      <c r="A14" s="27" t="inlineStr">
         <is>
           <t>200605</t>
         </is>
       </c>
-      <c r="B14" s="29" t="inlineStr">
+      <c r="B14" s="31" t="inlineStr">
         <is>
           <t>Martin Minsky</t>
         </is>
       </c>
-      <c r="C14" s="29" t="inlineStr">
+      <c r="C14" s="31" t="inlineStr">
         <is>
           <t>RS</t>
         </is>
       </c>
-      <c r="D14" s="26" t="n"/>
-      <c r="E14" s="30" t="inlineStr">
+      <c r="D14" s="28" t="n"/>
+      <c r="E14" s="32" t="inlineStr">
         <is>
           <t>4+</t>
         </is>
       </c>
-      <c r="F14" s="30" t="inlineStr">
+      <c r="F14" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G14" s="30" t="inlineStr">
+      <c r="G14" s="32" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="H14" s="30" t="inlineStr">
+      <c r="H14" s="32" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="I14" s="30" t="inlineStr">
+      <c r="I14" s="32" t="inlineStr">
         <is>
           <t>4+</t>
         </is>
       </c>
-      <c r="J14" s="30" t="inlineStr">
+      <c r="J14" s="32" t="inlineStr">
         <is>
           <t>4+</t>
         </is>
       </c>
-      <c r="K14" s="30" t="inlineStr">
+      <c r="K14" s="32" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="L14" s="30" t="inlineStr">
+      <c r="L14" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="M14" s="30" t="inlineStr">
+      <c r="M14" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="N14" s="30" t="inlineStr">
+      <c r="N14" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="O14" s="30" t="inlineStr">
+      <c r="O14" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="P14" s="30" t="inlineStr">
+      <c r="P14" s="32" t="inlineStr">
         <is>
           <t>5+</t>
         </is>
       </c>
-      <c r="Q14" s="30" t="inlineStr">
+      <c r="Q14" s="32" t="inlineStr">
         <is>
           <t>5-</t>
         </is>
       </c>
-      <c r="R14" s="30" t="inlineStr">
+      <c r="R14" s="32" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="S14" s="30" t="inlineStr">
+      <c r="S14" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
-      <c r="T14" s="30" t="inlineStr">
+      <c r="T14" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="U14" s="30" t="inlineStr">
+      <c r="U14" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22.4" r="15" s="16">
-      <c r="A15" s="25" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="15" s="17">
+      <c r="A15" s="27" t="inlineStr">
         <is>
           <t>200606</t>
         </is>
       </c>
-      <c r="B15" s="29" t="inlineStr">
+      <c r="B15" s="31" t="inlineStr">
         <is>
           <t>Nellie Nümann</t>
         </is>
       </c>
-      <c r="C15" s="29" t="inlineStr">
+      <c r="C15" s="31" t="inlineStr">
         <is>
           <t>RS</t>
         </is>
       </c>
-      <c r="D15" s="26" t="n"/>
-      <c r="E15" s="30" t="inlineStr">
+      <c r="D15" s="28" t="n"/>
+      <c r="E15" s="32" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="F15" s="30" t="inlineStr">
+      <c r="F15" s="32" t="inlineStr">
         <is>
           <t>5-</t>
         </is>
       </c>
-      <c r="G15" s="30" t="inlineStr">
+      <c r="G15" s="32" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="H15" s="30" t="inlineStr">
+      <c r="H15" s="32" t="inlineStr">
         <is>
           <t>2+</t>
         </is>
       </c>
-      <c r="I15" s="30" t="inlineStr">
+      <c r="I15" s="32" t="inlineStr">
         <is>
           <t>3+</t>
         </is>
       </c>
-      <c r="J15" s="30" t="inlineStr">
+      <c r="J15" s="32" t="inlineStr">
         <is>
           <t>3+</t>
         </is>
       </c>
-      <c r="K15" s="30" t="inlineStr">
+      <c r="K15" s="32" t="inlineStr">
         <is>
           <t>4-</t>
         </is>
       </c>
-      <c r="L15" s="30" t="inlineStr">
+      <c r="L15" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="M15" s="30" t="inlineStr">
+      <c r="M15" s="32" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="N15" s="30" t="inlineStr">
+      <c r="N15" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="O15" s="30" t="inlineStr">
+      <c r="O15" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="P15" s="30" t="inlineStr">
+      <c r="P15" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="Q15" s="30" t="inlineStr">
+      <c r="Q15" s="32" t="inlineStr">
         <is>
           <t>1-</t>
         </is>
       </c>
-      <c r="R15" s="30" t="inlineStr">
+      <c r="R15" s="32" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="S15" s="30" t="inlineStr">
+      <c r="S15" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="T15" s="30" t="inlineStr">
+      <c r="T15" s="32" t="inlineStr">
         <is>
           <t>1-</t>
         </is>
       </c>
-      <c r="U15" s="30" t="inlineStr">
+      <c r="U15" s="32" t="inlineStr">
         <is>
           <t>1+</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22.4" r="16" s="16">
-      <c r="A16" s="25" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="16" s="17">
+      <c r="A16" s="27" t="inlineStr">
         <is>
           <t>200851</t>
         </is>
       </c>
-      <c r="B16" s="29" t="inlineStr">
+      <c r="B16" s="31" t="inlineStr">
         <is>
           <t>Penelope Plaß</t>
         </is>
       </c>
-      <c r="C16" s="29" t="inlineStr">
+      <c r="C16" s="31" t="inlineStr">
         <is>
           <t>RS</t>
         </is>
       </c>
-      <c r="D16" s="26" t="n"/>
-      <c r="E16" s="30" t="inlineStr">
+      <c r="D16" s="28" t="n"/>
+      <c r="E16" s="32" t="inlineStr">
         <is>
           <t>1+</t>
         </is>
       </c>
-      <c r="F16" s="30" t="inlineStr">
+      <c r="F16" s="32" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="G16" s="30" t="inlineStr">
+      <c r="G16" s="32" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="H16" s="30" t="inlineStr">
+      <c r="H16" s="32" t="inlineStr">
         <is>
           <t>5+</t>
         </is>
       </c>
-      <c r="I16" s="30" t="inlineStr">
+      <c r="I16" s="32" t="inlineStr">
         <is>
           <t>4+</t>
         </is>
       </c>
-      <c r="J16" s="30" t="inlineStr">
+      <c r="J16" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="K16" s="30" t="inlineStr">
+      <c r="K16" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="L16" s="30" t="inlineStr">
+      <c r="L16" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="M16" s="30" t="inlineStr">
+      <c r="M16" s="32" t="inlineStr">
         <is>
           <t>1-</t>
         </is>
       </c>
-      <c r="N16" s="30" t="inlineStr">
+      <c r="N16" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="O16" s="30" t="inlineStr">
+      <c r="O16" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="P16" s="30" t="inlineStr">
+      <c r="P16" s="32" t="inlineStr">
         <is>
           <t>4-</t>
         </is>
       </c>
-      <c r="Q16" s="30" t="inlineStr">
+      <c r="Q16" s="32" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="R16" s="30" t="inlineStr">
+      <c r="R16" s="32" t="inlineStr">
         <is>
           <t>5-</t>
         </is>
       </c>
-      <c r="S16" s="30" t="inlineStr">
+      <c r="S16" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
-      <c r="T16" s="30" t="n"/>
-      <c r="U16" s="30" t="n"/>
+      <c r="T16" s="32" t="n"/>
+      <c r="U16" s="32" t="n"/>
     </row>
-    <row customHeight="1" ht="22.4" r="17" s="16">
-      <c r="A17" s="25" t="inlineStr">
+    <row customHeight="1" ht="22.4" r="17" s="17">
+      <c r="A17" s="27" t="inlineStr">
         <is>
           <t>200607</t>
         </is>
       </c>
-      <c r="B17" s="29" t="inlineStr">
+      <c r="B17" s="31" t="inlineStr">
         <is>
           <t>Irmgard Unstet</t>
         </is>
       </c>
-      <c r="C17" s="29" t="inlineStr">
+      <c r="C17" s="31" t="inlineStr">
         <is>
           <t>Gym</t>
         </is>
       </c>
-      <c r="D17" s="26" t="n"/>
-      <c r="E17" s="30" t="inlineStr">
+      <c r="D17" s="28" t="n"/>
+      <c r="E17" s="32" t="inlineStr">
         <is>
           <t>1+</t>
         </is>
       </c>
-      <c r="F17" s="30" t="inlineStr">
+      <c r="F17" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G17" s="30" t="inlineStr">
+      <c r="G17" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="H17" s="30" t="inlineStr">
+      <c r="H17" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I17" s="30" t="inlineStr">
+      <c r="I17" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="J17" s="30" t="inlineStr">
+      <c r="J17" s="32" t="inlineStr">
         <is>
           <t>3-</t>
         </is>
       </c>
-      <c r="K17" s="30" t="inlineStr">
+      <c r="K17" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="L17" s="30" t="inlineStr">
+      <c r="L17" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="M17" s="30" t="inlineStr">
+      <c r="M17" s="32" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="N17" s="30" t="inlineStr">
+      <c r="N17" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="O17" s="30" t="inlineStr">
+      <c r="O17" s="32" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="P17" s="30" t="inlineStr">
+      <c r="P17" s="32" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
-      <c r="Q17" s="30" t="inlineStr">
+      <c r="Q17" s="32" t="inlineStr">
         <is>
           <t>2-</t>
         </is>
       </c>
-      <c r="R17" s="30" t="inlineStr">
+      <c r="R17" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="S17" s="30" t="inlineStr">
+      <c r="S17" s="32" t="inlineStr">
         <is>
           <t>nt</t>
         </is>
       </c>
-      <c r="T17" s="30" t="inlineStr">
+      <c r="T17" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="U17" s="30" t="inlineStr">
+      <c r="U17" s="32" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22.4" r="18" s="16"/>
-    <row customHeight="1" ht="22.4" r="19" s="16"/>
-    <row customHeight="1" ht="22.4" r="20" s="16"/>
-    <row customHeight="1" ht="22.4" r="21" s="16"/>
-    <row customHeight="1" ht="22.4" r="22" s="16"/>
-    <row customHeight="1" ht="22.4" r="23" s="16"/>
-    <row customHeight="1" ht="22.4" r="24" s="16"/>
-    <row customHeight="1" ht="22.4" r="25" s="16"/>
-    <row customHeight="1" ht="22.4" r="26" s="16"/>
-    <row customHeight="1" ht="22.4" r="27" s="16"/>
-    <row customHeight="1" ht="22.4" r="28" s="16"/>
-    <row customHeight="1" ht="22.4" r="29" s="16"/>
-    <row customHeight="1" ht="22.4" r="30" s="16"/>
-    <row customHeight="1" ht="22.4" r="31" s="16"/>
-    <row customHeight="1" ht="22.4" r="32" s="16"/>
-    <row customHeight="1" ht="22.4" r="33" s="16"/>
-    <row customHeight="1" ht="22.4" r="34" s="16"/>
-    <row customHeight="1" ht="22.4" r="35" s="16"/>
-    <row customHeight="1" ht="22.4" r="36" s="16"/>
-    <row customHeight="1" ht="22.4" r="37" s="16"/>
-    <row customHeight="1" ht="22.4" r="38" s="16"/>
-    <row customHeight="1" ht="22.4" r="39" s="16"/>
-    <row customHeight="1" ht="22.4" r="40" s="16"/>
-    <row customHeight="1" ht="22.4" r="41" s="16"/>
-    <row customHeight="1" ht="22.4" r="42" s="16"/>
-    <row customHeight="1" ht="22.4" r="43" s="16"/>
-    <row customHeight="1" ht="22.4" r="44" s="16"/>
-    <row customHeight="1" ht="22.4" r="45" s="16"/>
-    <row customHeight="1" ht="22.4" r="46" s="16"/>
-    <row customHeight="1" ht="22.4" r="47" s="16"/>
-    <row customHeight="1" ht="22.4" r="48" s="16"/>
-    <row customHeight="1" ht="22.4" r="49" s="16"/>
-    <row customHeight="1" ht="22.4" r="50" s="16"/>
+    <row customHeight="1" ht="22.4" r="18" s="17"/>
+    <row customHeight="1" ht="22.4" r="19" s="17"/>
+    <row customHeight="1" ht="22.4" r="20" s="17"/>
+    <row customHeight="1" ht="22.4" r="21" s="17"/>
+    <row customHeight="1" ht="22.4" r="22" s="17"/>
+    <row customHeight="1" ht="22.4" r="23" s="17"/>
+    <row customHeight="1" ht="22.4" r="24" s="17"/>
+    <row customHeight="1" ht="22.4" r="25" s="17"/>
+    <row customHeight="1" ht="22.4" r="26" s="17"/>
+    <row customHeight="1" ht="22.4" r="27" s="17"/>
+    <row customHeight="1" ht="22.4" r="28" s="17"/>
+    <row customHeight="1" ht="22.4" r="29" s="17"/>
+    <row customHeight="1" ht="22.4" r="30" s="17"/>
+    <row customHeight="1" ht="22.4" r="31" s="17"/>
+    <row customHeight="1" ht="22.4" r="32" s="17"/>
+    <row customHeight="1" ht="22.4" r="33" s="17"/>
+    <row customHeight="1" ht="22.4" r="34" s="17"/>
+    <row customHeight="1" ht="22.4" r="35" s="17"/>
+    <row customHeight="1" ht="22.4" r="36" s="17"/>
+    <row customHeight="1" ht="22.4" r="37" s="17"/>
+    <row customHeight="1" ht="22.4" r="38" s="17"/>
+    <row customHeight="1" ht="22.4" r="39" s="17"/>
+    <row customHeight="1" ht="22.4" r="40" s="17"/>
+    <row customHeight="1" ht="22.4" r="41" s="17"/>
+    <row customHeight="1" ht="22.4" r="42" s="17"/>
+    <row customHeight="1" ht="22.4" r="43" s="17"/>
+    <row customHeight="1" ht="22.4" r="44" s="17"/>
+    <row customHeight="1" ht="22.4" r="45" s="17"/>
+    <row customHeight="1" ht="22.4" r="46" s="17"/>
+    <row customHeight="1" ht="22.4" r="47" s="17"/>
+    <row customHeight="1" ht="22.4" r="48" s="17"/>
+    <row customHeight="1" ht="22.4" r="49" s="17"/>
+    <row customHeight="1" ht="22.4" r="50" s="17"/>
   </sheetData>
   <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="0" pivotTables="1" scenarios="0" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:S1"/>
     <mergeCell ref="F2:S2"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="N3:P3"/>
+    <mergeCell ref="R3:S3"/>
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="N4:S4"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="0" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1" sqref="E9:AD50" type="list">
-      <formula1>"1+,1,1-,2+,2,2-,3+,3,3-,4+,4,4-,5+,5,5-,6,nb,nt,t,*"</formula1>
+      <formula1>"1+,1,1-,2+,2,2-,3+,3,3-,4+,4,4-,5+,5,5-,6,nb,nt,t,*,/"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>